<commit_message>
blabla- results of work with Nasko
</commit_message>
<xml_diff>
--- a/Administrative/Week4/ProPMoSCoW.xlsx
+++ b/Administrative/Week4/ProPMoSCoW.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\ProP\PROP-Project\Administrative\Week4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\FONTYSPRO\ProProject\PROP-Project\Administrative\Week4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>MoSCoW-list, ProP, febr. 2015</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Depeche Mode,Arctic Monkeys, Vampire Weekend, The black keys</t>
+  </si>
+  <si>
+    <t>Merchendise</t>
   </si>
 </sst>
 </file>
@@ -232,7 +235,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -248,9 +251,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office тема">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Оffice">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -288,7 +291,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Оffice">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -360,7 +363,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Оffice">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -513,20 +516,20 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.44140625" customWidth="1"/>
+    <col min="1" max="1" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -540,12 +543,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -553,7 +556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -561,7 +564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -569,7 +572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -577,7 +580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -585,7 +588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -593,7 +596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -601,7 +604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -609,7 +612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -617,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -625,7 +628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -633,7 +636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -641,7 +644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -649,7 +652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -657,12 +660,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -670,7 +673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -678,7 +681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -686,7 +689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -694,7 +697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -702,7 +705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -710,7 +713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -718,12 +721,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -731,7 +742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -739,7 +750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -747,7 +758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -755,17 +766,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>32</v>
       </c>
@@ -773,7 +784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>33</v>
       </c>
@@ -781,7 +792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -789,7 +800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>35</v>
       </c>
@@ -797,7 +808,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>36</v>
       </c>
@@ -805,7 +816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>37</v>
       </c>
@@ -813,7 +824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -821,7 +832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>39</v>
       </c>
@@ -829,7 +840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>40</v>
       </c>
@@ -837,7 +848,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>41</v>
       </c>
@@ -845,7 +856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>42</v>
       </c>
@@ -853,7 +864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>43</v>
       </c>
@@ -861,7 +872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>44</v>
       </c>
@@ -869,12 +880,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>46</v>
       </c>
@@ -882,7 +893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>47</v>
       </c>
@@ -890,7 +901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -898,7 +909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>49</v>
       </c>
@@ -906,7 +917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>50</v>
       </c>

</xml_diff>